<commit_message>
- updated input .xlsx and expected_out.csv - main.py: refactoring
</commit_message>
<xml_diff>
--- a/Vorplan Plan Q1-22 v4 - Für die Trainer.xlsx
+++ b/Vorplan Plan Q1-22 v4 - Für die Trainer.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">D E A D L I N E  :  28. November  2021</t>
   </si>
@@ -75,13 +75,13 @@
     <t>Frank</t>
   </si>
   <si>
-    <t>Spalte11</t>
+    <t>Kerstin</t>
   </si>
   <si>
-    <t>Spalte12</t>
+    <t>Stefan</t>
   </si>
   <si>
-    <t>Spalte13</t>
+    <t>Simon</t>
   </si>
   <si>
     <t>Spalte14</t>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">17:30 - 21:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerstin Hospi</t>
   </si>
   <si>
     <t xml:space="preserve">Eltern - Kind - Kurs</t>
@@ -324,13 +327,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <color theme="0"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -616,7 +619,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="3" fillId="5" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="6" fillId="6" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="7" fillId="6" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -635,13 +641,10 @@
     <xf fontId="0" fillId="0" borderId="5" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="6" fillId="6" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="7" fillId="6" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="8" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="7" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="9" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="7" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1555,14 +1558,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Tabelle5" ref="B4:J143">
-  <autoFilter ref="B4:J143">
-    <filterColumn colId="1">
-      <filters blank="1">
-        <dateGroupItem year="2021" month="10" day="2" dateTimeGrouping="day"/>
-        <dateGroupItem year="2021" month="10" day="3" dateTimeGrouping="day"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B4:J143"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Öffn." dataDxfId="0"/>
     <tableColumn id="2" name="Tag" dataDxfId="1"/>
@@ -1580,9 +1576,41 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" displayName="Tabelle1" ref="L4:AP143">
-  <autoFilter ref="L4:AP143"/>
+  <autoFilter ref="L4:AP142">
+    <filterColumn colId="0"/>
+    <filterColumn colId="1"/>
+    <filterColumn colId="2"/>
+    <filterColumn colId="3"/>
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
+    <filterColumn colId="7"/>
+    <filterColumn colId="8"/>
+    <filterColumn colId="9"/>
+    <filterColumn colId="10"/>
+    <filterColumn colId="11"/>
+    <filterColumn colId="12"/>
+    <filterColumn colId="13"/>
+    <filterColumn colId="14"/>
+    <filterColumn colId="15"/>
+    <filterColumn colId="16"/>
+    <filterColumn colId="17"/>
+    <filterColumn colId="18"/>
+    <filterColumn colId="19"/>
+    <filterColumn colId="20"/>
+    <filterColumn colId="21"/>
+    <filterColumn colId="22"/>
+    <filterColumn colId="23"/>
+    <filterColumn colId="24"/>
+    <filterColumn colId="25"/>
+    <filterColumn colId="26"/>
+    <filterColumn colId="27"/>
+    <filterColumn colId="28"/>
+    <filterColumn colId="29"/>
+    <filterColumn colId="30"/>
+  </autoFilter>
   <tableColumns count="31">
-    <tableColumn id="1" name="Marco" dataDxfId="9"/>
+    <tableColumn id="1" name="Marco" totalsRowLabel="Summary" dataDxfId="9"/>
     <tableColumn id="2" name="claudia" dataDxfId="10"/>
     <tableColumn id="3" name="Orsi" dataDxfId="11"/>
     <tableColumn id="4" name="Sosa" dataDxfId="12"/>
@@ -1592,9 +1620,9 @@
     <tableColumn id="8" name="Kathi" dataDxfId="16"/>
     <tableColumn id="9" name="Micha" dataDxfId="17"/>
     <tableColumn id="10" name="Frank" dataDxfId="18"/>
-    <tableColumn id="11" name="Spalte11" dataDxfId="19"/>
-    <tableColumn id="12" name="Spalte12" dataDxfId="20"/>
-    <tableColumn id="13" name="Spalte13" dataDxfId="21"/>
+    <tableColumn id="11" name="Kerstin" dataDxfId="19"/>
+    <tableColumn id="12" name="Stefan" dataDxfId="20"/>
+    <tableColumn id="13" name="Simon" dataDxfId="21"/>
     <tableColumn id="14" name="Spalte14" dataDxfId="22"/>
     <tableColumn id="15" name="Spalte15" dataDxfId="23"/>
     <tableColumn id="16" name="Spalte16" dataDxfId="24"/>
@@ -1612,7 +1640,7 @@
     <tableColumn id="28" name="Spalte28" dataDxfId="36"/>
     <tableColumn id="29" name="Spalte29" dataDxfId="37"/>
     <tableColumn id="30" name="Spalte30" dataDxfId="38"/>
-    <tableColumn id="31" name="Spalte31" dataDxfId="39"/>
+    <tableColumn id="31" name="Spalte31" totalsRowFunction="sum" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2114,10 +2142,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="U78" activeCellId="0" sqref="U78"/>
+      <selection activeCell="U14" activeCellId="0" sqref="U14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.880000000000001"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.7109375"/>
     <col customWidth="1" min="2" max="3" width="11.7109375"/>
@@ -2177,7 +2205,7 @@
       <c r="AO1" s="4"/>
       <c r="AP1" s="4"/>
     </row>
-    <row r="2" s="5" customFormat="1" ht="44.600000000000001">
+    <row r="2" s="5" customFormat="1" ht="45">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2285,13 +2313,13 @@
       <c r="U4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="16" t="s">
+      <c r="V4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="16" t="s">
+      <c r="W4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="16" t="s">
+      <c r="X4" s="15" t="s">
         <v>22</v>
       </c>
       <c r="Y4" s="16" t="s">
@@ -2493,7 +2521,9 @@
       <c r="U7" s="26"/>
       <c r="V7" s="26"/>
       <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
+      <c r="X7" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y7" s="26"/>
       <c r="Z7" s="26"/>
       <c r="AA7" s="26"/>
@@ -2513,7 +2543,7 @@
       <c r="AO7" s="26"/>
       <c r="AP7" s="27"/>
     </row>
-    <row r="8">
+    <row r="8" ht="14">
       <c r="B8" s="18" t="s">
         <v>46</v>
       </c>
@@ -2529,7 +2559,9 @@
       <c r="F8" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="30">
+        <v>44565</v>
+      </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
@@ -2545,9 +2577,13 @@
       <c r="S8" s="26"/>
       <c r="T8" s="26"/>
       <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
+      <c r="V8" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
+      <c r="X8" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y8" s="26"/>
       <c r="Z8" s="26"/>
       <c r="AA8" s="26"/>
@@ -2614,7 +2650,9 @@
       </c>
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
+      <c r="X9" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
       <c r="AA9" s="26"/>
@@ -2731,9 +2769,13 @@
         <v>18</v>
       </c>
       <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
+      <c r="V11" s="36" t="s">
+        <v>53</v>
+      </c>
       <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
+      <c r="X11" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y11" s="26"/>
       <c r="Z11" s="26"/>
       <c r="AA11" s="26"/>
@@ -2763,11 +2805,11 @@
       <c r="D12" s="20">
         <v>44569</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>53</v>
+      <c r="E12" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" s="30">
         <v>44569</v>
@@ -2777,7 +2819,7 @@
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
-      <c r="L12" s="37"/>
+      <c r="L12" s="38"/>
       <c r="M12" s="26"/>
       <c r="N12" s="25" t="s">
         <v>12</v>
@@ -2793,9 +2835,15 @@
       <c r="S12" s="26"/>
       <c r="T12" s="26"/>
       <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
+      <c r="V12" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="W12" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="X12" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y12" s="26"/>
       <c r="Z12" s="26"/>
       <c r="AA12" s="26"/>
@@ -2821,11 +2869,11 @@
       <c r="D13" s="20">
         <v>44569</v>
       </c>
-      <c r="E13" s="38" t="s">
-        <v>55</v>
+      <c r="E13" s="39" t="s">
+        <v>56</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G13" s="30">
         <v>44569</v>
@@ -2835,7 +2883,7 @@
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
-      <c r="L13" s="37"/>
+      <c r="L13" s="38"/>
       <c r="M13" s="26"/>
       <c r="N13" s="25" t="s">
         <v>12</v>
@@ -2853,7 +2901,9 @@
       <c r="U13" s="26"/>
       <c r="V13" s="26"/>
       <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
+      <c r="X13" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y13" s="26"/>
       <c r="Z13" s="26"/>
       <c r="AA13" s="26"/>
@@ -2879,11 +2929,11 @@
       <c r="D14" s="20">
         <v>44569</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="39" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G14" s="30">
         <v>44569</v>
@@ -2896,7 +2946,7 @@
       <c r="L14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="39"/>
+      <c r="M14" s="40"/>
       <c r="N14" s="25" t="s">
         <v>12</v>
       </c>
@@ -2913,9 +2963,15 @@
       <c r="U14" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
+      <c r="V14" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="X14" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y14" s="26"/>
       <c r="Z14" s="26"/>
       <c r="AA14" s="26"/>
@@ -2945,8 +3001,8 @@
       <c r="D15" s="20">
         <v>44570</v>
       </c>
-      <c r="E15" s="40" t="s">
-        <v>58</v>
+      <c r="E15" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>50</v>
@@ -3001,11 +3057,11 @@
       <c r="D16" s="20">
         <v>44570</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>58</v>
+      <c r="E16" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G16" s="30">
         <v>44570</v>
@@ -3055,8 +3111,8 @@
       <c r="D17" s="20">
         <v>44570</v>
       </c>
-      <c r="E17" s="41" t="s">
-        <v>60</v>
+      <c r="E17" s="42" t="s">
+        <v>61</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
@@ -3106,8 +3162,8 @@
       <c r="D18" s="20">
         <v>44571</v>
       </c>
-      <c r="E18" s="42" t="s">
-        <v>61</v>
+      <c r="E18" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
@@ -3117,7 +3173,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="25"/>
       <c r="M18" s="26"/>
-      <c r="N18" s="37"/>
+      <c r="N18" s="38"/>
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
@@ -3171,7 +3227,7 @@
       <c r="J19" s="31"/>
       <c r="L19" s="25"/>
       <c r="M19" s="26"/>
-      <c r="N19" s="37"/>
+      <c r="N19" s="38"/>
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
       <c r="Q19" s="26"/>
@@ -3213,8 +3269,8 @@
       <c r="D20" s="20">
         <v>44573</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>61</v>
+      <c r="E20" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
@@ -3224,7 +3280,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="25"/>
       <c r="M20" s="26"/>
-      <c r="N20" s="37"/>
+      <c r="N20" s="38"/>
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
       <c r="Q20" s="26"/>
@@ -3279,7 +3335,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="25"/>
       <c r="M21" s="26"/>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="38" t="s">
         <v>12</v>
       </c>
       <c r="O21" s="26"/>
@@ -3323,8 +3379,8 @@
       <c r="D22" s="20">
         <v>44575</v>
       </c>
-      <c r="E22" s="42" t="s">
-        <v>61</v>
+      <c r="E22" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
@@ -3333,7 +3389,7 @@
       <c r="J22" s="31"/>
       <c r="L22" s="25"/>
       <c r="M22" s="26"/>
-      <c r="N22" s="37"/>
+      <c r="N22" s="38"/>
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
@@ -3377,7 +3433,7 @@
         <v>48</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G23" s="20">
         <v>44576</v>
@@ -3389,7 +3445,7 @@
       <c r="J23" s="31"/>
       <c r="L23" s="25"/>
       <c r="M23" s="26"/>
-      <c r="N23" s="37"/>
+      <c r="N23" s="38"/>
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
@@ -3405,7 +3461,9 @@
       </c>
       <c r="V23" s="26"/>
       <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
+      <c r="X23" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y23" s="26"/>
       <c r="Z23" s="26"/>
       <c r="AA23" s="26"/>
@@ -3431,11 +3489,11 @@
       <c r="D24" s="20">
         <v>44576</v>
       </c>
-      <c r="E24" s="43" t="s">
-        <v>53</v>
+      <c r="E24" s="44" t="s">
+        <v>54</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G24" s="20">
         <v>44576</v>
@@ -3457,9 +3515,13 @@
       <c r="S24" s="26"/>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
+      <c r="V24" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
+      <c r="X24" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y24" s="26"/>
       <c r="Z24" s="26"/>
       <c r="AA24" s="26"/>
@@ -3485,11 +3547,11 @@
       <c r="D25" s="20">
         <v>44576</v>
       </c>
-      <c r="E25" s="44" t="s">
-        <v>63</v>
+      <c r="E25" s="45" t="s">
+        <v>64</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G25" s="20">
         <v>44576</v>
@@ -3513,7 +3575,9 @@
       <c r="U25" s="26"/>
       <c r="V25" s="26"/>
       <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
+      <c r="X25" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y25" s="26"/>
       <c r="Z25" s="26"/>
       <c r="AA25" s="26"/>
@@ -3543,8 +3607,8 @@
       <c r="D26" s="20">
         <v>44577</v>
       </c>
-      <c r="E26" s="45" t="s">
-        <v>58</v>
+      <c r="E26" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F26" s="29" t="s">
         <v>50</v>
@@ -3593,11 +3657,11 @@
       <c r="D27" s="20">
         <v>44577</v>
       </c>
-      <c r="E27" s="45" t="s">
-        <v>58</v>
+      <c r="E27" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G27" s="20">
         <v>44577</v>
@@ -3643,8 +3707,8 @@
       <c r="D28" s="20">
         <v>44577</v>
       </c>
-      <c r="E28" s="42" t="s">
-        <v>60</v>
+      <c r="E28" s="43" t="s">
+        <v>61</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
@@ -3694,8 +3758,8 @@
       <c r="D29" s="20">
         <v>44578</v>
       </c>
-      <c r="E29" s="42" t="s">
-        <v>61</v>
+      <c r="E29" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
@@ -3771,7 +3835,9 @@
       <c r="U30" s="26"/>
       <c r="V30" s="26"/>
       <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
+      <c r="X30" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y30" s="26"/>
       <c r="Z30" s="26"/>
       <c r="AA30" s="26"/>
@@ -3801,8 +3867,8 @@
       <c r="D31" s="20">
         <v>44580</v>
       </c>
-      <c r="E31" s="46" t="s">
-        <v>65</v>
+      <c r="E31" s="47" t="s">
+        <v>66</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>45</v>
@@ -3821,10 +3887,10 @@
         <v>11</v>
       </c>
       <c r="N31" s="25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P31" s="26"/>
       <c r="Q31" s="26"/>
@@ -3921,8 +3987,8 @@
       <c r="D33" s="20">
         <v>44582</v>
       </c>
-      <c r="E33" s="42" t="s">
-        <v>61</v>
+      <c r="E33" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
@@ -3971,11 +4037,11 @@
       <c r="D34" s="20">
         <v>44583</v>
       </c>
-      <c r="E34" s="43" t="s">
-        <v>53</v>
+      <c r="E34" s="44" t="s">
+        <v>54</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G34" s="20">
         <v>44583</v>
@@ -4001,7 +4067,9 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26"/>
-      <c r="X34" s="26"/>
+      <c r="X34" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y34" s="26"/>
       <c r="Z34" s="26"/>
       <c r="AA34" s="26"/>
@@ -4031,7 +4099,7 @@
         <v>51</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G35" s="20">
         <v>44583</v>
@@ -4044,13 +4112,13 @@
       <c r="L35" s="25"/>
       <c r="M35" s="26"/>
       <c r="N35" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O35" s="26"/>
       <c r="P35" s="26"/>
       <c r="Q35" s="26"/>
-      <c r="R35" s="47" t="s">
-        <v>69</v>
+      <c r="R35" s="36" t="s">
+        <v>70</v>
       </c>
       <c r="S35" s="26" t="s">
         <v>17</v>
@@ -4059,7 +4127,9 @@
       <c r="U35" s="26"/>
       <c r="V35" s="26"/>
       <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
+      <c r="X35" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y35" s="26"/>
       <c r="Z35" s="26"/>
       <c r="AA35" s="26"/>
@@ -4085,11 +4155,11 @@
       <c r="D36" s="20">
         <v>44583</v>
       </c>
-      <c r="E36" s="44" t="s">
-        <v>63</v>
+      <c r="E36" s="45" t="s">
+        <v>64</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G36" s="20">
         <v>44583</v>
@@ -4113,7 +4183,9 @@
       <c r="U36" s="26"/>
       <c r="V36" s="26"/>
       <c r="W36" s="26"/>
-      <c r="X36" s="26"/>
+      <c r="X36" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y36" s="26"/>
       <c r="Z36" s="26"/>
       <c r="AA36" s="26"/>
@@ -4143,8 +4215,8 @@
       <c r="D37" s="20">
         <v>44584</v>
       </c>
-      <c r="E37" s="45" t="s">
-        <v>58</v>
+      <c r="E37" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F37" s="29" t="s">
         <v>50</v>
@@ -4199,11 +4271,11 @@
       <c r="D38" s="20">
         <v>44584</v>
       </c>
-      <c r="E38" s="45" t="s">
-        <v>58</v>
+      <c r="E38" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G38" s="20">
         <v>44584</v>
@@ -4253,8 +4325,8 @@
       <c r="D39" s="20">
         <v>44584</v>
       </c>
-      <c r="E39" s="42" t="s">
-        <v>70</v>
+      <c r="E39" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F39" s="30"/>
       <c r="G39" s="30"/>
@@ -4304,8 +4376,8 @@
       <c r="D40" s="20">
         <v>44585</v>
       </c>
-      <c r="E40" s="42" t="s">
-        <v>61</v>
+      <c r="E40" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
@@ -4417,7 +4489,7 @@
         <v>48</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G42" s="20">
         <v>44587</v>
@@ -4440,9 +4512,13 @@
       <c r="S42" s="26"/>
       <c r="T42" s="26"/>
       <c r="U42" s="26"/>
-      <c r="V42" s="26"/>
+      <c r="V42" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
+      <c r="X42" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="Y42" s="26"/>
       <c r="Z42" s="26"/>
       <c r="AA42" s="26"/>
@@ -4529,8 +4605,8 @@
       <c r="D44" s="20">
         <v>44589</v>
       </c>
-      <c r="E44" s="42" t="s">
-        <v>61</v>
+      <c r="E44" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -4583,7 +4659,7 @@
         <v>48</v>
       </c>
       <c r="F45" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G45" s="20">
         <v>44590</v>
@@ -4611,9 +4687,15 @@
       <c r="U45" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="V45" s="26"/>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
+      <c r="V45" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W45" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="X45" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y45" s="26"/>
       <c r="Z45" s="26"/>
       <c r="AA45" s="26"/>
@@ -4639,11 +4721,11 @@
       <c r="D46" s="20">
         <v>44590</v>
       </c>
-      <c r="E46" s="43" t="s">
-        <v>53</v>
+      <c r="E46" s="44" t="s">
+        <v>54</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G46" s="20">
         <v>44590</v>
@@ -4667,7 +4749,9 @@
       <c r="U46" s="26"/>
       <c r="V46" s="26"/>
       <c r="W46" s="26"/>
-      <c r="X46" s="26"/>
+      <c r="X46" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y46" s="26"/>
       <c r="Z46" s="26"/>
       <c r="AA46" s="26"/>
@@ -4693,11 +4777,11 @@
       <c r="D47" s="20">
         <v>44590</v>
       </c>
-      <c r="E47" s="44" t="s">
-        <v>63</v>
+      <c r="E47" s="45" t="s">
+        <v>64</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G47" s="20">
         <v>44590</v>
@@ -4751,8 +4835,8 @@
       <c r="D48" s="20">
         <v>44591</v>
       </c>
-      <c r="E48" s="45" t="s">
-        <v>58</v>
+      <c r="E48" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F48" s="29" t="s">
         <v>50</v>
@@ -4801,11 +4885,11 @@
       <c r="D49" s="20">
         <v>44591</v>
       </c>
-      <c r="E49" s="45" t="s">
-        <v>58</v>
+      <c r="E49" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G49" s="20">
         <v>44591</v>
@@ -4851,8 +4935,8 @@
       <c r="D50" s="20">
         <v>44591</v>
       </c>
-      <c r="E50" s="42" t="s">
-        <v>70</v>
+      <c r="E50" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F50" s="23"/>
       <c r="G50" s="23"/>
@@ -4903,10 +4987,10 @@
         <v>44592</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G51" s="20">
         <v>44592</v>
@@ -4989,7 +5073,9 @@
       </c>
       <c r="V52" s="26"/>
       <c r="W52" s="26"/>
-      <c r="X52" s="26"/>
+      <c r="X52" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y52" s="26"/>
       <c r="Z52" s="26"/>
       <c r="AA52" s="26"/>
@@ -5020,7 +5106,7 @@
         <v>44594</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F53" s="29" t="s">
         <v>45</v>
@@ -5154,16 +5240,16 @@
       <c r="I55" s="30"/>
       <c r="J55" s="31"/>
       <c r="K55" s="13"/>
-      <c r="L55" s="39"/>
+      <c r="L55" s="40"/>
       <c r="M55" s="26"/>
-      <c r="N55" s="47" t="s">
-        <v>68</v>
+      <c r="N55" s="36" t="s">
+        <v>69</v>
       </c>
       <c r="O55" s="26"/>
       <c r="P55" s="26"/>
       <c r="Q55" s="26"/>
-      <c r="R55" s="47" t="s">
-        <v>69</v>
+      <c r="R55" s="36" t="s">
+        <v>70</v>
       </c>
       <c r="S55" s="26" t="s">
         <v>17</v>
@@ -5171,7 +5257,9 @@
       <c r="T55" s="26"/>
       <c r="U55" s="26"/>
       <c r="V55" s="26"/>
-      <c r="W55" s="26"/>
+      <c r="W55" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="X55" s="26"/>
       <c r="Y55" s="26"/>
       <c r="Z55" s="26"/>
@@ -5202,11 +5290,11 @@
       <c r="D56" s="20">
         <v>44597</v>
       </c>
-      <c r="E56" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="F56" s="41" t="s">
-        <v>74</v>
+      <c r="E56" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="42" t="s">
+        <v>75</v>
       </c>
       <c r="G56" s="20">
         <v>44597</v>
@@ -5220,7 +5308,7 @@
       <c r="O56" s="26"/>
       <c r="P56" s="26"/>
       <c r="Q56" s="26"/>
-      <c r="R56" s="47" t="s">
+      <c r="R56" s="36" t="s">
         <v>16</v>
       </c>
       <c r="S56" s="26"/>
@@ -5254,11 +5342,11 @@
       <c r="D57" s="20">
         <v>44597</v>
       </c>
-      <c r="E57" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F57" s="41" t="s">
-        <v>75</v>
+      <c r="E57" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" s="42" t="s">
+        <v>76</v>
       </c>
       <c r="G57" s="20">
         <v>44597</v>
@@ -5283,7 +5371,9 @@
       <c r="T57" s="26"/>
       <c r="U57" s="26"/>
       <c r="V57" s="26"/>
-      <c r="W57" s="26"/>
+      <c r="W57" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="X57" s="26"/>
       <c r="Y57" s="26"/>
       <c r="Z57" s="26"/>
@@ -5314,7 +5404,7 @@
         <v>48</v>
       </c>
       <c r="F58" s="49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G58" s="20">
         <v>44597</v>
@@ -5342,7 +5432,9 @@
       <c r="U58" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="V58" s="26"/>
+      <c r="V58" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="W58" s="26"/>
       <c r="X58" s="26"/>
       <c r="Y58" s="26"/>
@@ -5374,8 +5466,8 @@
       <c r="D59" s="20">
         <v>44598</v>
       </c>
-      <c r="E59" s="45" t="s">
-        <v>58</v>
+      <c r="E59" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F59" s="29" t="s">
         <v>50</v>
@@ -5426,11 +5518,11 @@
       <c r="D60" s="20">
         <v>44598</v>
       </c>
-      <c r="E60" s="45" t="s">
-        <v>58</v>
+      <c r="E60" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G60" s="20">
         <v>44598</v>
@@ -5478,8 +5570,8 @@
       <c r="D61" s="20">
         <v>44598</v>
       </c>
-      <c r="E61" s="42" t="s">
-        <v>70</v>
+      <c r="E61" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F61" s="30"/>
       <c r="G61" s="30"/>
@@ -5529,11 +5621,11 @@
       <c r="D62" s="20">
         <v>44599</v>
       </c>
-      <c r="E62" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="F62" s="41" t="s">
+      <c r="E62" s="47" t="s">
         <v>78</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>79</v>
       </c>
       <c r="G62" s="20">
         <v>44599</v>
@@ -5553,7 +5645,7 @@
       <c r="P62" s="26"/>
       <c r="Q62" s="26"/>
       <c r="R62" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S62" s="26"/>
       <c r="T62" s="26" t="s">
@@ -5650,8 +5742,8 @@
       <c r="D64" s="20">
         <v>44601</v>
       </c>
-      <c r="E64" s="42" t="s">
-        <v>61</v>
+      <c r="E64" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F64" s="30"/>
       <c r="G64" s="30"/>
@@ -5758,8 +5850,8 @@
       <c r="D66" s="20">
         <v>44603</v>
       </c>
-      <c r="E66" s="42" t="s">
-        <v>61</v>
+      <c r="E66" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F66" s="30"/>
       <c r="G66" s="30"/>
@@ -5808,11 +5900,11 @@
       <c r="D67" s="20">
         <v>44604</v>
       </c>
-      <c r="E67" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F67" s="41" t="s">
+      <c r="E67" s="44" t="s">
         <v>54</v>
+      </c>
+      <c r="F67" s="42" t="s">
+        <v>55</v>
       </c>
       <c r="G67" s="20">
         <v>44604</v>
@@ -5836,7 +5928,9 @@
       <c r="U67" s="26"/>
       <c r="V67" s="26"/>
       <c r="W67" s="26"/>
-      <c r="X67" s="26"/>
+      <c r="X67" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y67" s="26"/>
       <c r="Z67" s="26"/>
       <c r="AA67" s="26"/>
@@ -5866,7 +5960,7 @@
         <v>48</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G68" s="20">
         <v>44604</v>
@@ -5896,7 +5990,9 @@
       </c>
       <c r="V68" s="26"/>
       <c r="W68" s="26"/>
-      <c r="X68" s="26"/>
+      <c r="X68" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y68" s="26"/>
       <c r="Z68" s="26"/>
       <c r="AA68" s="26"/>
@@ -5922,11 +6018,11 @@
       <c r="D69" s="20">
         <v>44604</v>
       </c>
-      <c r="E69" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="F69" s="41" t="s">
+      <c r="E69" s="45" t="s">
         <v>64</v>
+      </c>
+      <c r="F69" s="42" t="s">
+        <v>65</v>
       </c>
       <c r="G69" s="20">
         <v>44604</v>
@@ -5950,7 +6046,9 @@
       <c r="U69" s="26"/>
       <c r="V69" s="26"/>
       <c r="W69" s="26"/>
-      <c r="X69" s="26"/>
+      <c r="X69" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y69" s="26"/>
       <c r="Z69" s="26"/>
       <c r="AA69" s="26"/>
@@ -5980,8 +6078,8 @@
       <c r="D70" s="20">
         <v>44605</v>
       </c>
-      <c r="E70" s="45" t="s">
-        <v>58</v>
+      <c r="E70" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F70" s="29" t="s">
         <v>50</v>
@@ -6032,11 +6130,11 @@
       <c r="D71" s="20">
         <v>44605</v>
       </c>
-      <c r="E71" s="45" t="s">
-        <v>58</v>
+      <c r="E71" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F71" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G71" s="20">
         <v>44605</v>
@@ -6082,8 +6180,8 @@
       <c r="D72" s="20">
         <v>44605</v>
       </c>
-      <c r="E72" s="42" t="s">
-        <v>70</v>
+      <c r="E72" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F72" s="30"/>
       <c r="G72" s="30"/>
@@ -6132,8 +6230,8 @@
       <c r="D73" s="20">
         <v>44606</v>
       </c>
-      <c r="E73" s="42" t="s">
-        <v>61</v>
+      <c r="E73" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F73" s="30"/>
       <c r="G73" s="30"/>
@@ -6212,7 +6310,9 @@
       <c r="U74" s="26"/>
       <c r="V74" s="26"/>
       <c r="W74" s="26"/>
-      <c r="X74" s="26"/>
+      <c r="X74" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y74" s="26"/>
       <c r="Z74" s="26"/>
       <c r="AA74" s="26"/>
@@ -6242,8 +6342,8 @@
       <c r="D75" s="20">
         <v>44608</v>
       </c>
-      <c r="E75" s="42" t="s">
-        <v>61</v>
+      <c r="E75" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F75" s="30"/>
       <c r="G75" s="20"/>
@@ -6348,11 +6448,11 @@
       <c r="D77" s="20">
         <v>44610</v>
       </c>
-      <c r="E77" s="46" t="s">
+      <c r="E77" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F77" s="42" t="s">
         <v>79</v>
-      </c>
-      <c r="F77" s="41" t="s">
-        <v>78</v>
       </c>
       <c r="G77" s="20">
         <v>44610</v>
@@ -6396,7 +6496,7 @@
       <c r="AO77" s="26"/>
       <c r="AP77" s="27"/>
     </row>
-    <row r="78" ht="13.85">
+    <row r="78">
       <c r="B78" s="18" t="s">
         <v>41</v>
       </c>
@@ -6406,11 +6506,11 @@
       <c r="D78" s="20">
         <v>44611</v>
       </c>
-      <c r="E78" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="F78" s="41" t="s">
-        <v>74</v>
+      <c r="E78" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F78" s="42" t="s">
+        <v>75</v>
       </c>
       <c r="G78" s="20">
         <v>44611</v>
@@ -6434,7 +6534,9 @@
       <c r="U78" s="26"/>
       <c r="V78" s="26"/>
       <c r="W78" s="26"/>
-      <c r="X78" s="26"/>
+      <c r="X78" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="Y78" s="26"/>
       <c r="Z78" s="26"/>
       <c r="AA78" s="26"/>
@@ -6460,11 +6562,11 @@
       <c r="D79" s="20">
         <v>44611</v>
       </c>
-      <c r="E79" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F79" s="41" t="s">
-        <v>75</v>
+      <c r="E79" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="F79" s="42" t="s">
+        <v>76</v>
       </c>
       <c r="G79" s="20">
         <v>44611</v>
@@ -6488,7 +6590,9 @@
       <c r="U79" s="26"/>
       <c r="V79" s="26"/>
       <c r="W79" s="26"/>
-      <c r="X79" s="26"/>
+      <c r="X79" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y79" s="26"/>
       <c r="Z79" s="26"/>
       <c r="AA79" s="26"/>
@@ -6517,8 +6621,8 @@
       <c r="E80" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F80" s="41" t="s">
-        <v>80</v>
+      <c r="F80" s="42" t="s">
+        <v>81</v>
       </c>
       <c r="G80" s="20">
         <v>44611</v>
@@ -6542,7 +6646,9 @@
       </c>
       <c r="V80" s="26"/>
       <c r="W80" s="26"/>
-      <c r="X80" s="26"/>
+      <c r="X80" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y80" s="26"/>
       <c r="Z80" s="26"/>
       <c r="AA80" s="26"/>
@@ -6572,8 +6678,8 @@
       <c r="D81" s="20">
         <v>44612</v>
       </c>
-      <c r="E81" s="45" t="s">
-        <v>58</v>
+      <c r="E81" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F81" s="29" t="s">
         <v>50</v>
@@ -6625,11 +6731,11 @@
       <c r="D82" s="20">
         <v>44612</v>
       </c>
-      <c r="E82" s="45" t="s">
-        <v>58</v>
+      <c r="E82" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F82" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G82" s="20">
         <v>44612</v>
@@ -6678,8 +6784,8 @@
       <c r="D83" s="20">
         <v>44612</v>
       </c>
-      <c r="E83" s="42" t="s">
-        <v>70</v>
+      <c r="E83" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F83" s="30"/>
       <c r="G83" s="30"/>
@@ -6731,8 +6837,8 @@
       <c r="E84" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F84" s="41" t="s">
-        <v>72</v>
+      <c r="F84" s="42" t="s">
+        <v>73</v>
       </c>
       <c r="G84" s="20">
         <v>44613</v>
@@ -6806,7 +6912,7 @@
       <c r="I85" s="30"/>
       <c r="J85" s="31"/>
       <c r="K85" s="3"/>
-      <c r="L85" s="39" t="s">
+      <c r="L85" s="40" t="s">
         <v>10</v>
       </c>
       <c r="M85" s="26"/>
@@ -6852,8 +6958,8 @@
       <c r="D86" s="20">
         <v>44615</v>
       </c>
-      <c r="E86" s="42" t="s">
-        <v>61</v>
+      <c r="E86" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F86" s="30"/>
       <c r="G86" s="20"/>
@@ -6960,8 +7066,8 @@
       <c r="D88" s="20">
         <v>44617</v>
       </c>
-      <c r="E88" s="42" t="s">
-        <v>61</v>
+      <c r="E88" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F88" s="30"/>
       <c r="G88" s="30"/>
@@ -7010,11 +7116,11 @@
       <c r="D89" s="20">
         <v>44618</v>
       </c>
-      <c r="E89" s="36" t="s">
-        <v>53</v>
+      <c r="E89" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="F89" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G89" s="20">
         <v>44618</v>
@@ -7038,7 +7144,9 @@
       <c r="U89" s="26"/>
       <c r="V89" s="26"/>
       <c r="W89" s="26"/>
-      <c r="X89" s="26"/>
+      <c r="X89" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y89" s="26"/>
       <c r="Z89" s="26"/>
       <c r="AA89" s="26"/>
@@ -7064,11 +7172,11 @@
       <c r="D90" s="20">
         <v>44618</v>
       </c>
-      <c r="E90" s="38" t="s">
-        <v>55</v>
+      <c r="E90" s="39" t="s">
+        <v>56</v>
       </c>
       <c r="F90" s="29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G90" s="20">
         <v>44618</v>
@@ -7094,7 +7202,9 @@
       <c r="U90" s="26"/>
       <c r="V90" s="26"/>
       <c r="W90" s="26"/>
-      <c r="X90" s="26"/>
+      <c r="X90" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y90" s="26"/>
       <c r="Z90" s="26"/>
       <c r="AA90" s="26"/>
@@ -7120,11 +7230,11 @@
       <c r="D91" s="20">
         <v>44618</v>
       </c>
-      <c r="E91" s="38" t="s">
+      <c r="E91" s="39" t="s">
         <v>48</v>
       </c>
       <c r="F91" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G91" s="20">
         <v>44618</v>
@@ -7152,7 +7262,9 @@
       </c>
       <c r="V91" s="26"/>
       <c r="W91" s="26"/>
-      <c r="X91" s="26"/>
+      <c r="X91" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y91" s="26"/>
       <c r="Z91" s="26"/>
       <c r="AA91" s="26"/>
@@ -7182,8 +7294,8 @@
       <c r="D92" s="20">
         <v>44619</v>
       </c>
-      <c r="E92" s="45" t="s">
-        <v>58</v>
+      <c r="E92" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F92" s="29" t="s">
         <v>50</v>
@@ -7234,11 +7346,11 @@
       <c r="D93" s="20">
         <v>44619</v>
       </c>
-      <c r="E93" s="45" t="s">
-        <v>58</v>
+      <c r="E93" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F93" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G93" s="20">
         <v>44619</v>
@@ -7287,8 +7399,8 @@
       <c r="D94" s="20">
         <v>44619</v>
       </c>
-      <c r="E94" s="42" t="s">
-        <v>60</v>
+      <c r="E94" s="43" t="s">
+        <v>61</v>
       </c>
       <c r="F94" s="30"/>
       <c r="G94" s="30"/>
@@ -7338,8 +7450,8 @@
       <c r="D95" s="20">
         <v>44620</v>
       </c>
-      <c r="E95" s="42" t="s">
-        <v>61</v>
+      <c r="E95" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F95" s="30"/>
       <c r="G95" s="30"/>
@@ -7414,7 +7526,9 @@
       <c r="U96" s="26"/>
       <c r="V96" s="26"/>
       <c r="W96" s="26"/>
-      <c r="X96" s="26"/>
+      <c r="X96" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y96" s="26"/>
       <c r="Z96" s="26"/>
       <c r="AA96" s="26"/>
@@ -7445,7 +7559,7 @@
         <v>44622</v>
       </c>
       <c r="E97" s="50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F97" s="30"/>
       <c r="G97" s="30"/>
@@ -7551,10 +7665,10 @@
         <v>44624</v>
       </c>
       <c r="E99" s="51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F99" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G99" s="20"/>
       <c r="H99" s="30"/>
@@ -7603,10 +7717,10 @@
         <v>44625</v>
       </c>
       <c r="E100" s="51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F100" s="52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G100" s="20"/>
       <c r="H100" s="30"/>
@@ -7654,8 +7768,8 @@
       <c r="E101" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F101" s="41" t="s">
-        <v>62</v>
+      <c r="F101" s="42" t="s">
+        <v>63</v>
       </c>
       <c r="G101" s="20">
         <v>44625</v>
@@ -7681,7 +7795,9 @@
       </c>
       <c r="V101" s="26"/>
       <c r="W101" s="26"/>
-      <c r="X101" s="26"/>
+      <c r="X101" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y101" s="26"/>
       <c r="Z101" s="26"/>
       <c r="AA101" s="26"/>
@@ -7712,10 +7828,10 @@
         <v>44626</v>
       </c>
       <c r="E102" s="51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F102" s="52" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G102" s="30"/>
       <c r="H102" s="30"/>
@@ -7760,8 +7876,8 @@
       <c r="D103" s="20">
         <v>44626</v>
       </c>
-      <c r="E103" s="45" t="s">
-        <v>58</v>
+      <c r="E103" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F103" s="29" t="s">
         <v>50</v>
@@ -7813,11 +7929,11 @@
       <c r="D104" s="20">
         <v>44626</v>
       </c>
-      <c r="E104" s="45" t="s">
-        <v>58</v>
+      <c r="E104" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F104" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G104" s="20">
         <v>44626</v>
@@ -7866,8 +7982,8 @@
       <c r="D105" s="20">
         <v>44626</v>
       </c>
-      <c r="E105" s="41" t="s">
-        <v>61</v>
+      <c r="E105" s="42" t="s">
+        <v>62</v>
       </c>
       <c r="F105" s="29"/>
       <c r="G105" s="30"/>
@@ -7916,11 +8032,11 @@
       <c r="D106" s="20">
         <v>44627</v>
       </c>
-      <c r="E106" s="46" t="s">
+      <c r="E106" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F106" s="42" t="s">
         <v>79</v>
-      </c>
-      <c r="F106" s="41" t="s">
-        <v>78</v>
       </c>
       <c r="G106" s="20">
         <v>44627</v>
@@ -7986,39 +8102,39 @@
       <c r="I107" s="30"/>
       <c r="J107" s="31"/>
       <c r="K107" s="3"/>
-      <c r="L107" s="39"/>
-      <c r="M107" s="37"/>
-      <c r="N107" s="37" t="s">
+      <c r="L107" s="40"/>
+      <c r="M107" s="38"/>
+      <c r="N107" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="O107" s="39"/>
-      <c r="P107" s="39"/>
-      <c r="Q107" s="39"/>
-      <c r="R107" s="39"/>
-      <c r="S107" s="39"/>
-      <c r="T107" s="39"/>
-      <c r="U107" s="39"/>
-      <c r="V107" s="39"/>
-      <c r="W107" s="39"/>
-      <c r="X107" s="39"/>
-      <c r="Y107" s="39"/>
-      <c r="Z107" s="39"/>
-      <c r="AA107" s="39"/>
-      <c r="AB107" s="39"/>
-      <c r="AC107" s="39"/>
-      <c r="AD107" s="39"/>
-      <c r="AE107" s="39"/>
-      <c r="AF107" s="39"/>
-      <c r="AG107" s="39"/>
-      <c r="AH107" s="39"/>
-      <c r="AI107" s="39"/>
-      <c r="AJ107" s="39"/>
-      <c r="AK107" s="39"/>
-      <c r="AL107" s="39"/>
-      <c r="AM107" s="39"/>
-      <c r="AN107" s="39"/>
-      <c r="AO107" s="39"/>
-      <c r="AP107" s="39"/>
+      <c r="O107" s="40"/>
+      <c r="P107" s="40"/>
+      <c r="Q107" s="40"/>
+      <c r="R107" s="40"/>
+      <c r="S107" s="40"/>
+      <c r="T107" s="40"/>
+      <c r="U107" s="40"/>
+      <c r="V107" s="40"/>
+      <c r="W107" s="40"/>
+      <c r="X107" s="40"/>
+      <c r="Y107" s="40"/>
+      <c r="Z107" s="40"/>
+      <c r="AA107" s="40"/>
+      <c r="AB107" s="40"/>
+      <c r="AC107" s="40"/>
+      <c r="AD107" s="40"/>
+      <c r="AE107" s="40"/>
+      <c r="AF107" s="40"/>
+      <c r="AG107" s="40"/>
+      <c r="AH107" s="40"/>
+      <c r="AI107" s="40"/>
+      <c r="AJ107" s="40"/>
+      <c r="AK107" s="40"/>
+      <c r="AL107" s="40"/>
+      <c r="AM107" s="40"/>
+      <c r="AN107" s="40"/>
+      <c r="AO107" s="40"/>
+      <c r="AP107" s="40"/>
     </row>
     <row r="108">
       <c r="B108" s="18" t="s">
@@ -8031,10 +8147,10 @@
         <v>44629</v>
       </c>
       <c r="E108" s="33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F108" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G108" s="20">
         <v>44629</v>
@@ -8151,7 +8267,7 @@
       <c r="E110" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F110" s="41" t="s">
+      <c r="F110" s="42" t="s">
         <v>45</v>
       </c>
       <c r="G110" s="30">
@@ -8178,7 +8294,9 @@
       <c r="U110" s="26"/>
       <c r="V110" s="26"/>
       <c r="W110" s="26"/>
-      <c r="X110" s="26"/>
+      <c r="X110" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y110" s="26"/>
       <c r="Z110" s="26"/>
       <c r="AA110" s="26"/>
@@ -8211,8 +8329,8 @@
       <c r="E111" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F111" s="41" t="s">
-        <v>54</v>
+      <c r="F111" s="42" t="s">
+        <v>55</v>
       </c>
       <c r="G111" s="20">
         <v>44632</v>
@@ -8238,7 +8356,9 @@
       <c r="U111" s="26"/>
       <c r="V111" s="26"/>
       <c r="W111" s="26"/>
-      <c r="X111" s="26"/>
+      <c r="X111" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y111" s="26"/>
       <c r="Z111" s="26"/>
       <c r="AA111" s="26"/>
@@ -8264,11 +8384,11 @@
       <c r="D112" s="20">
         <v>44632</v>
       </c>
-      <c r="E112" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="F112" s="41" t="s">
-        <v>85</v>
+      <c r="E112" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F112" s="42" t="s">
+        <v>86</v>
       </c>
       <c r="G112" s="20">
         <v>44632</v>
@@ -8292,7 +8412,9 @@
       </c>
       <c r="V112" s="26"/>
       <c r="W112" s="26"/>
-      <c r="X112" s="26"/>
+      <c r="X112" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y112" s="26"/>
       <c r="Z112" s="26"/>
       <c r="AA112" s="26"/>
@@ -8321,8 +8443,8 @@
       <c r="E113" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F113" s="41" t="s">
-        <v>80</v>
+      <c r="F113" s="42" t="s">
+        <v>81</v>
       </c>
       <c r="G113" s="20">
         <v>44632</v>
@@ -8341,7 +8463,7 @@
       <c r="P113" s="26"/>
       <c r="Q113" s="26"/>
       <c r="R113" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S113" s="26" t="s">
         <v>17</v>
@@ -8352,7 +8474,9 @@
       <c r="U113" s="26"/>
       <c r="V113" s="26"/>
       <c r="W113" s="26"/>
-      <c r="X113" s="26"/>
+      <c r="X113" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y113" s="26"/>
       <c r="Z113" s="26"/>
       <c r="AA113" s="26"/>
@@ -8382,8 +8506,8 @@
       <c r="D114" s="20">
         <v>44633</v>
       </c>
-      <c r="E114" s="45" t="s">
-        <v>58</v>
+      <c r="E114" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F114" s="29" t="s">
         <v>50</v>
@@ -8433,11 +8557,11 @@
       <c r="D115" s="20">
         <v>44633</v>
       </c>
-      <c r="E115" s="45" t="s">
-        <v>58</v>
+      <c r="E115" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F115" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G115" s="20">
         <v>44633</v>
@@ -8484,8 +8608,8 @@
       <c r="D116" s="20">
         <v>44633</v>
       </c>
-      <c r="E116" s="42" t="s">
-        <v>70</v>
+      <c r="E116" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F116" s="30"/>
       <c r="G116" s="30"/>
@@ -8534,8 +8658,8 @@
       <c r="D117" s="20">
         <v>44634</v>
       </c>
-      <c r="E117" s="42" t="s">
-        <v>61</v>
+      <c r="E117" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F117" s="30"/>
       <c r="G117" s="30"/>
@@ -8612,7 +8736,9 @@
       </c>
       <c r="V118" s="26"/>
       <c r="W118" s="26"/>
-      <c r="X118" s="26"/>
+      <c r="X118" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y118" s="26"/>
       <c r="Z118" s="26"/>
       <c r="AA118" s="26"/>
@@ -8642,8 +8768,8 @@
       <c r="D119" s="20">
         <v>44636</v>
       </c>
-      <c r="E119" s="42" t="s">
-        <v>61</v>
+      <c r="E119" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F119" s="30"/>
       <c r="G119" s="20"/>
@@ -8748,8 +8874,8 @@
       <c r="D121" s="20">
         <v>44638</v>
       </c>
-      <c r="E121" s="42" t="s">
-        <v>61</v>
+      <c r="E121" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F121" s="30"/>
       <c r="G121" s="30"/>
@@ -8798,11 +8924,11 @@
       <c r="D122" s="20">
         <v>44639</v>
       </c>
-      <c r="E122" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F122" s="41" t="s">
+      <c r="E122" s="44" t="s">
         <v>54</v>
+      </c>
+      <c r="F122" s="42" t="s">
+        <v>55</v>
       </c>
       <c r="G122" s="20">
         <v>44639</v>
@@ -8826,7 +8952,9 @@
       <c r="U122" s="26"/>
       <c r="V122" s="26"/>
       <c r="W122" s="26"/>
-      <c r="X122" s="26"/>
+      <c r="X122" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y122" s="26"/>
       <c r="Z122" s="26"/>
       <c r="AA122" s="26"/>
@@ -8855,8 +8983,8 @@
       <c r="E123" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F123" s="41" t="s">
-        <v>62</v>
+      <c r="F123" s="42" t="s">
+        <v>63</v>
       </c>
       <c r="G123" s="20">
         <v>44639</v>
@@ -8886,7 +9014,9 @@
       </c>
       <c r="V123" s="26"/>
       <c r="W123" s="26"/>
-      <c r="X123" s="26"/>
+      <c r="X123" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y123" s="26"/>
       <c r="Z123" s="26"/>
       <c r="AA123" s="26"/>
@@ -8912,11 +9042,11 @@
       <c r="D124" s="20">
         <v>44639</v>
       </c>
-      <c r="E124" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="F124" s="41" t="s">
+      <c r="E124" s="45" t="s">
         <v>64</v>
+      </c>
+      <c r="F124" s="42" t="s">
+        <v>65</v>
       </c>
       <c r="G124" s="20">
         <v>44639</v>
@@ -8940,7 +9070,9 @@
       </c>
       <c r="V124" s="26"/>
       <c r="W124" s="26"/>
-      <c r="X124" s="26"/>
+      <c r="X124" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="Y124" s="26"/>
       <c r="Z124" s="26"/>
       <c r="AA124" s="26"/>
@@ -8970,8 +9102,8 @@
       <c r="D125" s="20">
         <v>44640</v>
       </c>
-      <c r="E125" s="45" t="s">
-        <v>58</v>
+      <c r="E125" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F125" s="29" t="s">
         <v>50</v>
@@ -9021,11 +9153,11 @@
       <c r="D126" s="20">
         <v>44640</v>
       </c>
-      <c r="E126" s="45" t="s">
-        <v>58</v>
+      <c r="E126" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F126" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G126" s="20">
         <v>44640</v>
@@ -9074,8 +9206,8 @@
       <c r="D127" s="20">
         <v>44640</v>
       </c>
-      <c r="E127" s="42" t="s">
-        <v>70</v>
+      <c r="E127" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F127" s="30"/>
       <c r="G127" s="30"/>
@@ -9127,8 +9259,8 @@
       <c r="E128" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F128" s="41" t="s">
-        <v>72</v>
+      <c r="F128" s="42" t="s">
+        <v>73</v>
       </c>
       <c r="G128" s="20">
         <v>44641</v>
@@ -9157,9 +9289,15 @@
       </c>
       <c r="T128" s="26"/>
       <c r="U128" s="26"/>
-      <c r="V128" s="26"/>
-      <c r="W128" s="26"/>
-      <c r="X128" s="26"/>
+      <c r="V128" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W128" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="X128" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="Y128" s="26"/>
       <c r="Z128" s="26"/>
       <c r="AA128" s="26"/>
@@ -9214,7 +9352,9 @@
       <c r="S129" s="26"/>
       <c r="T129" s="26"/>
       <c r="U129" s="26"/>
-      <c r="V129" s="26"/>
+      <c r="V129" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="W129" s="26"/>
       <c r="X129" s="26"/>
       <c r="Y129" s="26"/>
@@ -9246,11 +9386,11 @@
       <c r="D130" s="20">
         <v>44643</v>
       </c>
-      <c r="E130" s="46" t="s">
+      <c r="E130" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F130" s="42" t="s">
         <v>79</v>
-      </c>
-      <c r="F130" s="41" t="s">
-        <v>78</v>
       </c>
       <c r="G130" s="20">
         <v>44643</v>
@@ -9359,7 +9499,7 @@
         <v>44645</v>
       </c>
       <c r="E132" s="53" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="30"/>
@@ -9412,7 +9552,7 @@
         <v>48</v>
       </c>
       <c r="F133" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G133" s="20">
         <v>44646</v>
@@ -9440,9 +9580,15 @@
       <c r="U133" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="V133" s="26"/>
-      <c r="W133" s="26"/>
-      <c r="X133" s="26"/>
+      <c r="V133" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W133" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="X133" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y133" s="26"/>
       <c r="Z133" s="26"/>
       <c r="AA133" s="26"/>
@@ -9468,11 +9614,11 @@
       <c r="D134" s="20">
         <v>44646</v>
       </c>
-      <c r="E134" s="43" t="s">
-        <v>53</v>
+      <c r="E134" s="44" t="s">
+        <v>54</v>
       </c>
       <c r="F134" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G134" s="20">
         <v>44646</v>
@@ -9500,7 +9646,9 @@
       <c r="U134" s="26"/>
       <c r="V134" s="26"/>
       <c r="W134" s="26"/>
-      <c r="X134" s="26"/>
+      <c r="X134" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y134" s="26"/>
       <c r="Z134" s="26"/>
       <c r="AA134" s="26"/>
@@ -9526,11 +9674,11 @@
       <c r="D135" s="20">
         <v>44646</v>
       </c>
-      <c r="E135" s="44" t="s">
-        <v>63</v>
+      <c r="E135" s="45" t="s">
+        <v>64</v>
       </c>
       <c r="F135" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G135" s="20">
         <v>44646</v>
@@ -9554,7 +9702,9 @@
       <c r="U135" s="26"/>
       <c r="V135" s="26"/>
       <c r="W135" s="26"/>
-      <c r="X135" s="26"/>
+      <c r="X135" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y135" s="26"/>
       <c r="Z135" s="26"/>
       <c r="AA135" s="26"/>
@@ -9584,8 +9734,8 @@
       <c r="D136" s="20">
         <v>44647</v>
       </c>
-      <c r="E136" s="45" t="s">
-        <v>58</v>
+      <c r="E136" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F136" s="29" t="s">
         <v>50</v>
@@ -9635,11 +9785,11 @@
       <c r="D137" s="20">
         <v>44647</v>
       </c>
-      <c r="E137" s="45" t="s">
-        <v>58</v>
+      <c r="E137" s="46" t="s">
+        <v>59</v>
       </c>
       <c r="F137" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G137" s="20">
         <v>44647</v>
@@ -9686,8 +9836,8 @@
       <c r="D138" s="20">
         <v>44647</v>
       </c>
-      <c r="E138" s="42" t="s">
-        <v>70</v>
+      <c r="E138" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="F138" s="23"/>
       <c r="G138" s="30"/>
@@ -9736,8 +9886,8 @@
       <c r="D139" s="20">
         <v>44648</v>
       </c>
-      <c r="E139" s="42" t="s">
-        <v>61</v>
+      <c r="E139" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F139" s="30"/>
       <c r="G139" s="30"/>
@@ -9812,9 +9962,13 @@
       <c r="U140" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="V140" s="26"/>
+      <c r="V140" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="W140" s="26"/>
-      <c r="X140" s="26"/>
+      <c r="X140" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="Y140" s="26"/>
       <c r="Z140" s="26"/>
       <c r="AA140" s="26"/>
@@ -9844,8 +9998,8 @@
       <c r="D141" s="20">
         <v>44650</v>
       </c>
-      <c r="E141" s="42" t="s">
-        <v>61</v>
+      <c r="E141" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="F141" s="30"/>
       <c r="G141" s="20"/>
@@ -9951,7 +10105,7 @@
         <v>44652</v>
       </c>
       <c r="E143" s="57" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F143" s="58"/>
       <c r="G143" s="56"/>

</xml_diff>